<commit_message>
Add new variables to data and update report
</commit_message>
<xml_diff>
--- a/data/raw-data/exampledata.xlsx
+++ b/data/raw-data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{EA1B0400-91DC-4479-905F-9A91D902E8D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72AD26FB-F75E-4473-83AB-2A6D4F4425BE}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="945" windowWidth="48840" windowHeight="21645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7425" yWindow="0" windowWidth="13170" windowHeight="10905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -72,6 +72,33 @@
   </si>
   <si>
     <t>identified gender (male/female/other)</t>
+  </si>
+  <si>
+    <t>hours_sleep</t>
+  </si>
+  <si>
+    <t>eye_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brown </t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>numbers of hours a person sleeps per night</t>
+  </si>
+  <si>
+    <t>numeric (hours)</t>
+  </si>
+  <si>
+    <t>eye color category</t>
+  </si>
+  <si>
+    <t>brown, blue, green</t>
   </si>
 </sst>
 </file>
@@ -398,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,8 +443,14 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
@@ -427,8 +460,14 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
@@ -438,8 +477,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -449,8 +494,14 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>7.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
@@ -460,8 +511,14 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
@@ -471,8 +528,14 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -482,8 +545,14 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
@@ -493,8 +562,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
@@ -504,8 +579,14 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
@@ -515,8 +596,14 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
@@ -526,16 +613,28 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>6.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
@@ -545,8 +644,14 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
@@ -556,8 +661,14 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
@@ -566,6 +677,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -575,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +749,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>